<commit_message>
Guia Api Generix fix
</commit_message>
<xml_diff>
--- a/Guia_Api_Facturas_Generix.xlsx
+++ b/Guia_Api_Facturas_Generix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\layuso\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://generixgrouponline-my.sharepoint.com/personal/icastro_generixgroup_com/Documents/Documentos/GITHUB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010EF652-DD21-44E7-ABE9-A00A0A7ADC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{010EF652-DD21-44E7-ABE9-A00A0A7ADC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{042D9953-D251-46F7-99C5-DCDF2FD1DBBA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Esquema General" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="541">
   <si>
     <t>JSON</t>
   </si>
@@ -1614,36 +1614,12 @@
     <t>2.2.5.1.12.</t>
   </si>
   <si>
-    <t>2.2.5.1.12.1.</t>
-  </si>
-  <si>
-    <t>2.2.5.1.12.1.1.</t>
-  </si>
-  <si>
-    <t>2.2.5.1.12.1.2.</t>
-  </si>
-  <si>
-    <t>2.2.5.1.12.1.3.</t>
-  </si>
-  <si>
-    <t>2.2.5.1.12.1.3.1.</t>
-  </si>
-  <si>
-    <t>2.2.5.1.12.1.4.</t>
-  </si>
-  <si>
-    <t>2.2.5.1.12.1.4.1.</t>
-  </si>
-  <si>
     <t>2.2.5.1.13.</t>
   </si>
   <si>
     <t>2.2.5.1.13.1.</t>
   </si>
   <si>
-    <t>2.2.5.1.13.2.</t>
-  </si>
-  <si>
     <t>2.2.5.1.14.</t>
   </si>
   <si>
@@ -1687,6 +1663,33 @@
   </si>
   <si>
     <t>2.2.7.1.1.5.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.13.1.1.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.13.1.2.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.13.1.3.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.13.1.3.1.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.13.1.4.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.13.1.4.1.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.14.1.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.14.2.</t>
+  </si>
+  <si>
+    <t>2.2.5.1.15.</t>
   </si>
 </sst>
 </file>
@@ -2568,8 +2571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -5871,8 +5874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25333C4E-FCEB-4BCB-A95F-5DF88E54B42A}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7484,7 +7487,7 @@
     <row r="74" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15"/>
       <c r="B74" s="15" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>62</v>
@@ -7504,7 +7507,7 @@
     <row r="75" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15"/>
       <c r="B75" s="15" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>63</v>
@@ -7526,7 +7529,7 @@
     <row r="76" spans="1:8" ht="108" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="15"/>
       <c r="B76" s="15" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>64</v>
@@ -7548,7 +7551,7 @@
     <row r="77" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="15"/>
       <c r="B77" s="15" t="s">
-        <v>517</v>
+        <v>533</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>65</v>
@@ -7572,7 +7575,7 @@
     <row r="78" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="15"/>
       <c r="B78" s="15" t="s">
-        <v>518</v>
+        <v>534</v>
       </c>
       <c r="C78" s="15" t="s">
         <v>66</v>
@@ -7594,7 +7597,7 @@
     <row r="79" spans="1:8" ht="36" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="15"/>
       <c r="B79" s="15" t="s">
-        <v>519</v>
+        <v>535</v>
       </c>
       <c r="C79" s="15" t="s">
         <v>37</v>
@@ -7618,7 +7621,7 @@
     <row r="80" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="15"/>
       <c r="B80" s="15" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>67</v>
@@ -7640,7 +7643,7 @@
     <row r="81" spans="1:8" ht="36" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="15"/>
       <c r="B81" s="15" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="C81" s="15" t="s">
         <v>37</v>
@@ -7664,7 +7667,7 @@
     <row r="82" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="15"/>
       <c r="B82" s="15" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>104</v>
@@ -7686,7 +7689,7 @@
     <row r="83" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="15"/>
       <c r="B83" s="15" t="s">
-        <v>523</v>
+        <v>538</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>58</v>
@@ -7708,7 +7711,7 @@
     <row r="84" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="15"/>
       <c r="B84" s="15" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>59</v>
@@ -7730,7 +7733,7 @@
     <row r="85" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="15"/>
       <c r="B85" s="15" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>105</v>
@@ -7774,7 +7777,7 @@
     <row r="87" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="15"/>
       <c r="B87" s="15" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>107</v>
@@ -7796,7 +7799,7 @@
     <row r="88" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="15"/>
       <c r="B88" s="15" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>108</v>
@@ -7818,7 +7821,7 @@
     <row r="89" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="15"/>
       <c r="B89" s="15" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>109</v>
@@ -7840,7 +7843,7 @@
     <row r="90" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15"/>
       <c r="B90" s="15" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="C90" s="15" t="s">
         <v>110</v>
@@ -7862,7 +7865,7 @@
     <row r="91" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15"/>
       <c r="B91" s="15" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>111</v>
@@ -7884,7 +7887,7 @@
     <row r="92" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15"/>
       <c r="B92" s="15" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="C92" s="15" t="s">
         <v>112</v>
@@ -7906,7 +7909,7 @@
     <row r="93" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15"/>
       <c r="B93" s="15" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>113</v>
@@ -7950,7 +7953,7 @@
     <row r="95" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="15"/>
       <c r="B95" s="15" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>115</v>
@@ -7972,7 +7975,7 @@
     <row r="96" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
       <c r="B96" s="15" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C96" s="15" t="s">
         <v>116</v>
@@ -7994,7 +7997,7 @@
     <row r="97" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="15"/>
       <c r="B97" s="15" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="C97" s="15" t="s">
         <v>117</v>
@@ -8016,7 +8019,7 @@
     <row r="98" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15"/>
       <c r="B98" s="15" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>118</v>
@@ -8038,7 +8041,7 @@
     <row r="99" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="15"/>
       <c r="B99" s="15" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="C99" s="15" t="s">
         <v>119</v>
@@ -8060,7 +8063,7 @@
     <row r="100" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="15"/>
       <c r="B100" s="15" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="C100" s="15" t="s">
         <v>120</v>
@@ -8082,7 +8085,7 @@
     <row r="101" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
       <c r="B101" s="15" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="C101" s="15" t="s">
         <v>121</v>
@@ -8111,21 +8114,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010059947A54AABC264B9B6A1395610EB9E4" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="039196c1875697d49709999e09f36296">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="669b3db3-d5a4-4d30-a460-f1a7bf62d82d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9472c2359e272d42a2ac2df94db4dd7c" ns2:_="">
     <xsd:import namespace="669b3db3-d5a4-4d30-a460-f1a7bf62d82d"/>
@@ -8269,24 +8257,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DACEA6D3-E19D-4B7E-B8E4-FC2FFCAA4342}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7511AB4F-EDCE-4C8F-9114-F29EE1FED04D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7010204-F282-4DB8-BAA4-6B407FACE274}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8302,4 +8288,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7511AB4F-EDCE-4C8F-9114-F29EE1FED04D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DACEA6D3-E19D-4B7E-B8E4-FC2FFCAA4342}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to new version
</commit_message>
<xml_diff>
--- a/Guia_Api_Facturas_Generix.xlsx
+++ b/Guia_Api_Facturas_Generix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://generixgrouponline-my.sharepoint.com/personal/icastro_generixgroup_com/Documents/Documentos/GitHub/GenerixCyC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:1_{010EF652-DD21-44E7-ABE9-A00A0A7ADC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6505001-0138-46C3-AF46-3F460229ADA0}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="13_ncr:1_{010EF652-DD21-44E7-ABE9-A00A0A7ADC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33397D9E-2C46-45FA-819E-618215A416A7}"/>
   <bookViews>
-    <workbookView xWindow="14685" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22428" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Esquema General" sheetId="1" r:id="rId1"/>
@@ -4470,8 +4470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B13C99-BA63-4783-81FE-9F858A27BFD2}">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -4669,7 +4669,7 @@
       <c r="B11" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="43" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="43" t="s">
@@ -4691,7 +4691,7 @@
       <c r="B12" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="43" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="43" t="s">
@@ -4713,7 +4713,7 @@
       <c r="B13" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="43" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="43" t="s">
@@ -4735,7 +4735,7 @@
       <c r="B14" s="20" t="s">
         <v>397</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="43" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="43" t="s">
@@ -4757,7 +4757,7 @@
       <c r="B15" s="20" t="s">
         <v>398</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="43" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="43" t="s">
@@ -4779,7 +4779,7 @@
       <c r="B16" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="43" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="43" t="s">
@@ -4801,7 +4801,7 @@
       <c r="B17" s="20" t="s">
         <v>400</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="43" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="43" t="s">
@@ -4823,7 +4823,7 @@
       <c r="B18" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="43" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="43" t="s">
@@ -4845,7 +4845,7 @@
       <c r="B19" s="20" t="s">
         <v>402</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="43" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="43" t="s">
@@ -4867,7 +4867,7 @@
       <c r="B20" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="43" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="43" t="s">
@@ -4889,7 +4889,7 @@
       <c r="B21" s="20" t="s">
         <v>404</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="43" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="43" t="s">
@@ -4911,7 +4911,7 @@
       <c r="B22" s="20" t="s">
         <v>405</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="43" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="43" t="s">
@@ -4933,7 +4933,7 @@
       <c r="B23" s="20" t="s">
         <v>406</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="43" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="43" t="s">
@@ -4955,7 +4955,7 @@
       <c r="B24" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="43" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="43" t="s">
@@ -4977,7 +4977,7 @@
       <c r="B25" s="20" t="s">
         <v>408</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="43" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="43" t="s">
@@ -4999,7 +4999,7 @@
       <c r="B26" s="20" t="s">
         <v>409</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="43" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="43" t="s">
@@ -5021,7 +5021,7 @@
       <c r="B27" s="20" t="s">
         <v>410</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="43" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="43" t="s">
@@ -5043,7 +5043,7 @@
       <c r="B28" s="20" t="s">
         <v>411</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="43" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="43" t="s">
@@ -5065,7 +5065,7 @@
       <c r="B29" s="20" t="s">
         <v>412</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="43" t="s">
         <v>564</v>
       </c>
       <c r="D29" s="43" t="s">
@@ -5087,7 +5087,7 @@
       <c r="B30" s="20" t="s">
         <v>522</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="43" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="25" t="s">
@@ -6234,7 +6234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25333C4E-FCEB-4BCB-A95F-5DF88E54B42A}">
   <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -8758,21 +8758,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010059947A54AABC264B9B6A1395610EB9E4" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="039196c1875697d49709999e09f36296">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="669b3db3-d5a4-4d30-a460-f1a7bf62d82d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9472c2359e272d42a2ac2df94db4dd7c" ns2:_="">
     <xsd:import namespace="669b3db3-d5a4-4d30-a460-f1a7bf62d82d"/>
@@ -8916,24 +8901,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7511AB4F-EDCE-4C8F-9114-F29EE1FED04D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DACEA6D3-E19D-4B7E-B8E4-FC2FFCAA4342}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7010204-F282-4DB8-BAA4-6B407FACE274}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8949,4 +8932,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DACEA6D3-E19D-4B7E-B8E4-FC2FFCAA4342}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7511AB4F-EDCE-4C8F-9114-F29EE1FED04D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>